<commit_message>
se agregaron todos los instrumentos existentes
</commit_message>
<xml_diff>
--- a/TP2/GUI-Synth/PROGRESO.xlsx
+++ b/TP2/GUI-Synth/PROGRESO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\ASSD\TP2\GUI-Synth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E8662F-CE0E-4419-A409-923DBD34B8E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5A5313-221F-4F98-88FD-AF0AE1F35083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{087B934F-F985-43E7-8A7E-BB411BA2E593}"/>
+    <workbookView xWindow="17010" yWindow="2580" windowWidth="21600" windowHeight="11385" xr2:uid="{087B934F-F985-43E7-8A7E-BB411BA2E593}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>INSTRUMENT</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>TOTAL DE TOTALES</t>
+  </si>
+  <si>
+    <t>N° of inst</t>
   </si>
 </sst>
 </file>
@@ -162,7 +165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,8 +190,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -248,12 +257,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -261,53 +307,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,7 +686,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,27 +695,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="G1" s="22" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -666,83 +727,112 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
         <f>C2/3 + D2/3 + E2/3</f>
         <v>1</v>
       </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4">
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3">
         <f>C3/3 + D3/3 + E3/3</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G3" s="2">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="5">
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18">
+        <v>1</v>
+      </c>
+      <c r="E4" s="18">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12">
         <f>C4/6 + C5/6 + D4/3 + E4/3</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="18">
+        <v>7</v>
+      </c>
+      <c r="I4" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="18"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="5"/>
-      <c r="I5" s="19">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="18"/>
+      <c r="I5" s="15">
         <f>AVERAGE(B28,F17)</f>
-        <v>0.2638888888888889</v>
+        <v>0.4</v>
       </c>
       <c r="J5" s="16"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="6">
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
         <f>C6/3 + D6/3 + E6/3</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -751,39 +841,44 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="5">
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="12">
         <f>C7/9 + C8/9 + C9/9 + D7/3 + E7/3</f>
         <v>0.33333333333333331</v>
       </c>
+      <c r="G7" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="5"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="5"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -792,45 +887,44 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4">
-        <f>C10/3 + D10/3 + E10/3</f>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="12">
+        <f>C10/9 + C11/9 + C12/9 + D10/3 + E10/3</f>
         <v>0.33333333333333331</v>
       </c>
+      <c r="G10" s="18">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4">
-        <f t="shared" ref="F11:F16" si="0">C11/3 + D11/3 + E11/3</f>
-        <v>0.33333333333333331</v>
-      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4">
-        <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
-      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -839,19 +933,22 @@
       <c r="C13" s="1">
         <v>1</v>
       </c>
-      <c r="D13" s="3">
-        <v>1</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <f>C13/3 + D13/3 + E13/3</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -860,19 +957,22 @@
       <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="3">
-        <v>1</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" ref="F14:F16" si="0">C14/3 + D14/3 + E14/3</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -881,19 +981,22 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="3">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4">
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="G15" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -902,110 +1005,123 @@
       <c r="C16" s="1">
         <v>1</v>
       </c>
-      <c r="D16" s="3">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1</v>
-      </c>
-      <c r="F16" s="4">
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="G16" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="15">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="11">
         <f>AVERAGE(F2:F16)</f>
-        <v>0.52777777777777779</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+        <v>0.8</v>
+      </c>
+      <c r="G17" s="23">
+        <f>MAX(G2:G16)+1</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="8">
         <f>AVERAGE(B20:B27)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="17">
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="G4:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
carga trucha guido mirala
</commit_message>
<xml_diff>
--- a/TP2/GUI-Synth/PROGRESO.xlsx
+++ b/TP2/GUI-Synth/PROGRESO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\ASSD\TP2\GUI-Synth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5A5313-221F-4F98-88FD-AF0AE1F35083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90740C3-44B1-408C-9CF7-919F551806DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17010" yWindow="2580" windowWidth="21600" windowHeight="11385" xr2:uid="{087B934F-F985-43E7-8A7E-BB411BA2E593}"/>
   </bookViews>
@@ -686,7 +686,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="J37" sqref="J36:J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,7 +803,7 @@
       <c r="G5" s="18"/>
       <c r="I5" s="15">
         <f>AVERAGE(B28,F17)</f>
-        <v>0.4</v>
+        <v>0.43333333333333329</v>
       </c>
       <c r="J5" s="16"/>
     </row>
@@ -841,11 +841,13 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="18"/>
+      <c r="D7" s="18">
+        <v>1</v>
+      </c>
       <c r="E7" s="18"/>
       <c r="F7" s="12">
         <f>C7/9 + C8/9 + C9/9 + D7/3 + E7/3</f>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G7" s="18">
         <v>1</v>
@@ -887,11 +889,13 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="19"/>
+      <c r="D10" s="19">
+        <v>1</v>
+      </c>
       <c r="E10" s="19"/>
       <c r="F10" s="12">
         <f>C10/9 + C11/9 + C12/9 + D10/3 + E10/3</f>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G10" s="18">
         <v>2</v>
@@ -1029,7 +1033,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="11">
         <f>AVERAGE(F2:F16)</f>
-        <v>0.8</v>
+        <v>0.86666666666666659</v>
       </c>
       <c r="G17" s="23">
         <f>MAX(G2:G16)+1</f>

</xml_diff>

<commit_message>
I WANT IT THAT WAY :musical_note:
</commit_message>
<xml_diff>
--- a/TP2/GUI-Synth/PROGRESO.xlsx
+++ b/TP2/GUI-Synth/PROGRESO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\ASSD\TP2\GUI-Synth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59518DFB-C764-4435-8A20-F0D581301A99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982CCE33-9957-4680-8A53-586634A8913E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15555" yWindow="1965" windowWidth="21600" windowHeight="11385" xr2:uid="{087B934F-F985-43E7-8A7E-BB411BA2E593}"/>
   </bookViews>
@@ -299,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -307,9 +307,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -322,9 +319,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -341,9 +335,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -366,6 +357,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -686,7 +689,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,30 +698,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -733,7 +736,7 @@
       <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="22">
         <f>C2/3 + D2/3 + E2/3</f>
         <v>1</v>
       </c>
@@ -742,7 +745,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -757,7 +760,7 @@
       <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="22">
         <f>C3/3 + D3/3 + E3/3</f>
         <v>1</v>
       </c>
@@ -766,7 +769,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -775,44 +778,44 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="14">
-        <v>1</v>
-      </c>
-      <c r="E4" s="14">
-        <v>1</v>
-      </c>
-      <c r="F4" s="15">
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+      <c r="F4" s="23">
         <f>C4/6 + C5/6 + D4/3 + E4/3</f>
         <v>1</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="12">
         <v>7</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="21"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="14"/>
-      <c r="I5" s="22">
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="12"/>
+      <c r="I5" s="19">
         <f>AVERAGE(B28,F17)</f>
-        <v>0.5</v>
-      </c>
-      <c r="J5" s="23"/>
+        <v>0.5625</v>
+      </c>
+      <c r="J5" s="20"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -827,7 +830,7 @@
       <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="22">
         <f>C6/3 + D6/3 + E6/3</f>
         <v>1</v>
       </c>
@@ -836,7 +839,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -845,48 +848,48 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="14">
-        <v>1</v>
-      </c>
-      <c r="E7" s="14">
-        <v>1</v>
-      </c>
-      <c r="F7" s="15">
+      <c r="D7" s="12">
+        <v>1</v>
+      </c>
+      <c r="E7" s="12">
+        <v>1</v>
+      </c>
+      <c r="F7" s="23">
         <f>C7/9 + C8/9 + C9/9 + D7/3 + E7/3</f>
         <v>1</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="14"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="14"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -895,48 +898,48 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="17">
-        <v>1</v>
-      </c>
-      <c r="E10" s="17">
-        <v>1</v>
-      </c>
-      <c r="F10" s="15">
+      <c r="D10" s="14">
+        <v>1</v>
+      </c>
+      <c r="E10" s="14">
+        <v>1</v>
+      </c>
+      <c r="F10" s="23">
         <f>C10/9 + C11/9 + C12/9 + D10/3 + E10/3</f>
         <v>1</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -951,7 +954,7 @@
       <c r="E13" s="2">
         <v>1</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="22">
         <f>C13/3 + D13/3 + E13/3</f>
         <v>1</v>
       </c>
@@ -960,7 +963,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -975,7 +978,7 @@
       <c r="E14" s="2">
         <v>1</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="22">
         <f t="shared" ref="F14:F16" si="0">C14/3 + D14/3 + E14/3</f>
         <v>1</v>
       </c>
@@ -984,7 +987,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -999,7 +1002,7 @@
       <c r="E15" s="2">
         <v>1</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="22">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1008,7 +1011,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1023,7 +1026,7 @@
       <c r="E16" s="2">
         <v>1</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="22">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1032,87 +1035,101 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="11">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="9">
         <f>AVERAGE(F2:F16)</f>
         <v>1</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="11">
         <f>MAX(G2:G16)+1</f>
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="24">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="24">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="21">
         <f>AVERAGE(B20:B27)</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
noseporque pero el audio no se reproduce
</commit_message>
<xml_diff>
--- a/TP2/GUI-Synth/PROGRESO.xlsx
+++ b/TP2/GUI-Synth/PROGRESO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\ASSD\TP2\GUI-Synth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982CCE33-9957-4680-8A53-586634A8913E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AF3363-B245-4225-941D-CB68DD27B95D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15555" yWindow="1965" windowWidth="21600" windowHeight="11385" xr2:uid="{087B934F-F985-43E7-8A7E-BB411BA2E593}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{087B934F-F985-43E7-8A7E-BB411BA2E593}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>INSTRUMENT</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>N° of inst</t>
+  </si>
+  <si>
+    <t>Play WAV</t>
   </si>
 </sst>
 </file>
@@ -299,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -332,10 +335,34 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -347,28 +374,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -686,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C679E9-F08B-48AB-81D5-D49350C6C4CB}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,7 +745,7 @@
       <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="13">
         <f>C2/3 + D2/3 + E2/3</f>
         <v>1</v>
       </c>
@@ -760,7 +769,7 @@
       <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="13">
         <f>C3/3 + D3/3 + E3/3</f>
         <v>1</v>
       </c>
@@ -769,7 +778,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -778,41 +787,41 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="12">
-        <v>1</v>
-      </c>
-      <c r="E4" s="12">
-        <v>1</v>
-      </c>
-      <c r="F4" s="23">
+      <c r="D4" s="20">
+        <v>1</v>
+      </c>
+      <c r="E4" s="20">
+        <v>1</v>
+      </c>
+      <c r="F4" s="21">
         <f>C4/6 + C5/6 + D4/3 + E4/3</f>
         <v>1</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="20">
         <v>7</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="18"/>
+      <c r="J4" s="16"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="12"/>
-      <c r="I5" s="19">
-        <f>AVERAGE(B28,F17)</f>
-        <v>0.5625</v>
-      </c>
-      <c r="J5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="20"/>
+      <c r="I5" s="17">
+        <f>AVERAGE(B29,F17)</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -830,7 +839,7 @@
       <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="13">
         <f>C6/3 + D6/3 + E6/3</f>
         <v>1</v>
       </c>
@@ -839,7 +848,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -848,48 +857,48 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="12">
-        <v>1</v>
-      </c>
-      <c r="E7" s="12">
-        <v>1</v>
-      </c>
-      <c r="F7" s="23">
+      <c r="D7" s="20">
+        <v>1</v>
+      </c>
+      <c r="E7" s="20">
+        <v>1</v>
+      </c>
+      <c r="F7" s="21">
         <f>C7/9 + C8/9 + C9/9 + D7/3 + E7/3</f>
         <v>1</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -898,45 +907,45 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="14">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14">
-        <v>1</v>
-      </c>
-      <c r="F10" s="23">
+      <c r="D10" s="22">
+        <v>1</v>
+      </c>
+      <c r="E10" s="22">
+        <v>1</v>
+      </c>
+      <c r="F10" s="21">
         <f>C10/9 + C11/9 + C12/9 + D10/3 + E10/3</f>
         <v>1</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="12"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="12"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -954,7 +963,7 @@
       <c r="E13" s="2">
         <v>1</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="13">
         <f>C13/3 + D13/3 + E13/3</f>
         <v>1</v>
       </c>
@@ -978,7 +987,7 @@
       <c r="E14" s="2">
         <v>1</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="13">
         <f t="shared" ref="F14:F16" si="0">C14/3 + D14/3 + E14/3</f>
         <v>1</v>
       </c>
@@ -1002,7 +1011,7 @@
       <c r="E15" s="2">
         <v>1</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1026,7 +1035,7 @@
       <c r="E16" s="2">
         <v>1</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1063,7 +1072,7 @@
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="24">
+      <c r="B20" s="14">
         <v>0</v>
       </c>
     </row>
@@ -1071,7 +1080,7 @@
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="24">
+      <c r="B21" s="14">
         <v>1</v>
       </c>
     </row>
@@ -1079,7 +1088,7 @@
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="24">
+      <c r="B22" s="14">
         <v>0</v>
       </c>
     </row>
@@ -1087,7 +1096,7 @@
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="24">
+      <c r="B23" s="14">
         <v>0</v>
       </c>
     </row>
@@ -1095,51 +1104,53 @@
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="24">
+      <c r="B24" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="24">
+      <c r="B26" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="24">
+      <c r="B28" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="21">
-        <f>AVERAGE(B20:B27)</f>
-        <v>0.125</v>
+      <c r="B29" s="12">
+        <f>AVERAGE(B20:B28)</f>
+        <v>0.16666666666666666</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="G4:G5"/>
     <mergeCell ref="G10:G12"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="A10:A12"/>
@@ -1151,6 +1162,12 @@
     <mergeCell ref="E10:E12"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="F7:F9"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="G4:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
COMPLETEN EL EXCEL POR FAVOR
</commit_message>
<xml_diff>
--- a/TP2/GUI-Synth/PROGRESO.xlsx
+++ b/TP2/GUI-Synth/PROGRESO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\New-ASSD\TP2\GUI-Synth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD95EDE3-3780-4212-8A79-F439768A13CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B484B21-47F8-4E84-9317-FA35AF5D7CB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{087B934F-F985-43E7-8A7E-BB411BA2E593}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
   <si>
     <t>INSTRUMENT</t>
   </si>
@@ -189,6 +189,69 @@
   </si>
   <si>
     <t>N° of wind.</t>
+  </si>
+  <si>
+    <t>Min.</t>
+  </si>
+  <si>
+    <t>Max.</t>
+  </si>
+  <si>
+    <t>DDM</t>
+  </si>
+  <si>
+    <t>Elemento</t>
+  </si>
+  <si>
+    <t>Param.</t>
+  </si>
+  <si>
+    <t>Instrum.</t>
+  </si>
+  <si>
+    <t>Guitar</t>
+  </si>
+  <si>
+    <t>E. Guitar</t>
+  </si>
+  <si>
+    <t>Effects</t>
+  </si>
+  <si>
+    <t>Eco</t>
+  </si>
+  <si>
+    <t>Time Eco</t>
+  </si>
+  <si>
+    <t>Decay Factor</t>
+  </si>
+  <si>
+    <t>Reverb.</t>
+  </si>
+  <si>
+    <t>Mix Factor</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>Gauss</t>
+  </si>
+  <si>
+    <t>Stand. Dev.</t>
+  </si>
+  <si>
+    <t>Exp.</t>
+  </si>
+  <si>
+    <t>Decay</t>
+  </si>
+  <si>
+    <t>Kaiser</t>
+  </si>
+  <si>
+    <t>Beta</t>
   </si>
 </sst>
 </file>
@@ -219,7 +282,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +313,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -353,7 +428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -410,12 +485,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -425,17 +518,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -752,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C679E9-F08B-48AB-81D5-D49350C6C4CB}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +851,7 @@
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -787,7 +874,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -810,8 +897,23 @@
       <c r="G2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -834,9 +936,20 @@
       <c r="G3" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="M3" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -845,43 +958,59 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="19">
-        <v>1</v>
-      </c>
-      <c r="E4" s="19">
-        <v>1</v>
-      </c>
-      <c r="F4" s="20">
+      <c r="D4" s="26">
+        <v>1</v>
+      </c>
+      <c r="E4" s="26">
+        <v>1</v>
+      </c>
+      <c r="F4" s="27">
         <f>C4/6 + C5/6 + D4/3 + E4/3</f>
         <v>1</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="26">
         <v>7</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="26"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="J4" s="22"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="19"/>
-      <c r="I5" s="27">
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="26"/>
+      <c r="I5" s="23">
         <f>AVERAGE(F17,B29,G31)</f>
         <v>0.81481481481481488</v>
       </c>
-      <c r="J5" s="28"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="24"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -904,9 +1033,16 @@
       <c r="G6" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="M6" s="32"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -915,48 +1051,71 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="19">
-        <v>1</v>
-      </c>
-      <c r="E7" s="19">
-        <v>1</v>
-      </c>
-      <c r="F7" s="20">
+      <c r="D7" s="26">
+        <v>1</v>
+      </c>
+      <c r="E7" s="26">
+        <v>1</v>
+      </c>
+      <c r="F7" s="27">
         <f>C7/9 + C8/9 + C9/9 + D7/3 + E7/3</f>
         <v>1</v>
       </c>
-      <c r="G7" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="G7" s="26">
+        <v>1</v>
+      </c>
+      <c r="M7" s="32"/>
+      <c r="N7" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="19"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="26"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="19"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="26"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -965,47 +1124,72 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="22">
-        <v>1</v>
-      </c>
-      <c r="E10" s="22">
-        <v>1</v>
-      </c>
-      <c r="F10" s="20">
+      <c r="D10" s="28">
+        <v>1</v>
+      </c>
+      <c r="E10" s="28">
+        <v>1</v>
+      </c>
+      <c r="F10" s="27">
         <f>C10/9 + C11/9 + C12/9 + D10/3 + E10/3</f>
         <v>1</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="19"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="26"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="19"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="26"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="O12" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1028,8 +1212,19 @@
       <c r="G13" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M13" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="N13" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="O13" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1052,8 +1247,15 @@
       <c r="G14" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M14" s="32"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1076,8 +1278,17 @@
       <c r="G15" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M15" s="32"/>
+      <c r="N15" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="O15" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -1100,8 +1311,15 @@
       <c r="G16" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M16" s="32"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>22</v>
       </c>
@@ -1117,8 +1335,30 @@
         <f>MAX(G2:G16)+1</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M17" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="N17" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="O17" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M18" s="32"/>
+      <c r="N18" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="O18" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -1134,8 +1374,17 @@
       <c r="H19" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M19" s="32"/>
+      <c r="N19" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="O19" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
@@ -1152,7 +1401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -1168,11 +1417,8 @@
       <c r="H21" s="18">
         <v>1</v>
       </c>
-      <c r="K21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -1191,11 +1437,8 @@
       <c r="H22" s="18">
         <v>2</v>
       </c>
-      <c r="K22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
@@ -1211,11 +1454,8 @@
       <c r="H23" s="18">
         <v>3</v>
       </c>
-      <c r="K23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
@@ -1231,8 +1471,11 @@
       <c r="H24" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>34</v>
       </c>
@@ -1248,8 +1491,11 @@
       <c r="H25" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>29</v>
       </c>
@@ -1265,8 +1511,11 @@
       <c r="H26" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1283,7 +1532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1300,7 +1549,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>22</v>
       </c>
@@ -1318,7 +1567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F30" s="5" t="s">
         <v>43</v>
       </c>
@@ -1329,7 +1578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F31" s="8" t="s">
         <v>22</v>
       </c>
@@ -1343,13 +1592,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="G4:G5"/>
+  <mergeCells count="25">
+    <mergeCell ref="M17:M19"/>
+    <mergeCell ref="M3:M12"/>
+    <mergeCell ref="N4:N6"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="M13:M16"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="N15:N16"/>
     <mergeCell ref="G10:G12"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="A10:A12"/>
@@ -1361,6 +1612,12 @@
     <mergeCell ref="E10:E12"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="F7:F9"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="G4:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>